<commit_message>
Remove green formatting for word_change
</commit_message>
<xml_diff>
--- a/resource/outfile_test_compare_expected.xlsx
+++ b/resource/outfile_test_compare_expected.xlsx
@@ -14441,17 +14441,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -34843,14 +34833,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>0.4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>0.4</formula>
       <formula>0.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>